<commit_message>
added info to CAD_BOM, added info to README.
</commit_message>
<xml_diff>
--- a/Piezo-Nanopositioner-V1/CAD Design/CAD BOM.xlsx
+++ b/Piezo-Nanopositioner-V1/CAD Design/CAD BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radur\Projects\Hacker Fab\Hardware\Piezo-Nanopositioner-V1\CAD Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1BA6BE-9600-4EA9-9B05-6167862AB0AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82817F2-ACC2-47A9-ADA9-A100A35AC926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Part</t>
   </si>
@@ -73,16 +73,33 @@
   </si>
   <si>
     <t>Linear Bearing</t>
+  </si>
+  <si>
+    <t>1 (pack of 100)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -117,15 +134,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -407,15 +427,14 @@
   <dimension ref="B2:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="61.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
@@ -436,8 +455,11 @@
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
@@ -447,8 +469,11 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
@@ -483,6 +508,11 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{C8E24F93-2F39-4EF7-9EBA-96951FF60006}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{0F5CFEEC-802C-4268-A36D-9D6D921CFCE1}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>